<commit_message>
Update average daily mortality to summer average
</commit_message>
<xml_diff>
--- a/input_data/impact_functions/annual_deaths.xlsx
+++ b/input_data/impact_functions/annual_deaths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliestalhanske/python_projects/heat_mortality_impact/input_data/impact_functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BAB43E-55C4-ED4D-8E6D-100F119B08F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4E4C32-D3C3-864E-824A-36ECD5C792F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="19200" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="500" windowWidth="19200" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>annual_deaths</t>
-  </si>
-  <si>
     <t>Over 75</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Genève</t>
+  </si>
+  <si>
+    <t>daily_deaths</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,9 +193,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -490,7 +487,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -504,9 +501,9 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -521,17 +518,17 @@
         <v>27</v>
       </c>
       <c r="B2" s="2">
-        <f>D2*C$2</f>
-        <v>48840.063999999998</v>
-      </c>
-      <c r="C2" s="7">
+        <f>D2*C$2/365</f>
+        <v>133.80839452054795</v>
+      </c>
+      <c r="C2" s="6">
         <v>0.72799999999999998</v>
       </c>
       <c r="D2" s="3">
         <v>67088</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -539,15 +536,15 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B28" si="0">D3*C$2</f>
-        <v>3479.8399999999997</v>
+        <f t="shared" ref="B3:B55" si="0">D3*C$2/365</f>
+        <v>9.5338082191780806</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3">
         <v>4780</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -556,14 +553,14 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" si="0"/>
-        <v>334.15199999999999</v>
+        <v>0.91548493150684929</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3">
         <v>459</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -572,14 +569,14 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
-        <v>99.736000000000004</v>
+        <v>0.27324931506849315</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="3">
         <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -588,14 +585,14 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
-        <v>1780.6879999999999</v>
+        <v>4.8785972602739722</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3">
         <v>2446</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -604,14 +601,14 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>1512.056</v>
+        <v>4.1426191780821915</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="3">
         <v>2077</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -620,14 +617,14 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
-        <v>6880.3279999999995</v>
+        <v>18.850213698630135</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3">
         <v>9451</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -636,30 +633,30 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
-        <v>1498.2239999999999</v>
+        <v>4.1047232876712325</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="3">
         <v>2058</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>2464.2799999999997</v>
+        <v>6.7514520547945196</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="3">
         <v>3385</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -668,14 +665,14 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>264.26400000000001</v>
+        <v>0.7240109589041096</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="3">
         <v>363</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -684,14 +681,14 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>1302.3920000000001</v>
+        <v>3.5681972602739727</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="3">
         <v>1789</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -700,14 +697,14 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
-        <v>495.03999999999996</v>
+        <v>1.3562739726027395</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="3">
         <v>680</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -716,14 +713,14 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>2285.92</v>
+        <v>6.2627945205479456</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="3">
         <v>3140</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -732,14 +729,14 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>1165.528</v>
+        <v>3.1932273972602738</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="3">
         <v>1601</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -748,14 +745,14 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>219.12799999999999</v>
+        <v>0.60035068493150678</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="3">
         <v>301</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -764,14 +761,14 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>187.82399999999998</v>
+        <v>0.51458630136986294</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="3">
         <v>258</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -780,14 +777,14 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>563.47199999999998</v>
+        <v>1.5437589041095889</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="3">
         <v>774</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -796,14 +793,14 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
-        <v>838.65599999999995</v>
+        <v>2.2976876712328766</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="3">
         <v>1152</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -812,14 +809,14 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
-        <v>1793.7919999999999</v>
+        <v>4.9144986301369862</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="3">
         <v>2464</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -828,14 +825,14 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" si="0"/>
-        <v>2824.64</v>
+        <v>7.7387397260273971</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="3">
         <v>3880</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -844,14 +841,14 @@
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
-        <v>1504.7760000000001</v>
+        <v>4.1226739726027395</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="3">
         <v>2067</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -860,14 +857,14 @@
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
-        <v>2294.6559999999999</v>
+        <v>6.2867287671232877</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="3">
         <v>3152</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -876,14 +873,14 @@
       </c>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
-        <v>235.87199999999999</v>
+        <v>0.64622465753424652</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3">
         <v>324</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -892,14 +889,14 @@
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
-        <v>1983.0719999999999</v>
+        <v>5.4330739726027391</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="3">
         <v>2724</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -908,14 +905,14 @@
       </c>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
-        <v>4186</v>
+        <v>11.468493150684932</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="3">
         <v>5750</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -924,14 +921,14 @@
       </c>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
-        <v>592.59199999999998</v>
+        <v>1.6235397260273972</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="3">
         <v>814</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -940,448 +937,448 @@
       </c>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
-        <v>8053.1359999999995</v>
+        <v>22.06338630136986</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="3">
         <v>11062</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="4">
-        <f>D29*C$29</f>
-        <v>18247.936000000002</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
+        <v>133.80839452054795</v>
+      </c>
+      <c r="C29" s="4">
         <v>0.27200000000000002</v>
       </c>
       <c r="D29" s="3">
         <v>67088</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="4">
-        <f t="shared" ref="B30:B55" si="1">D30*C$29</f>
-        <v>1300.1600000000001</v>
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
+        <v>9.5338082191780806</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3">
         <v>4780</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>124.84800000000001</v>
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91548493150684929</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3">
         <v>459</v>
       </c>
       <c r="E31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="4">
-        <f t="shared" si="1"/>
-        <v>37.264000000000003</v>
+      <c r="B32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27324931506849315</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3">
         <v>137</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="4">
-        <f t="shared" si="1"/>
-        <v>665.31200000000001</v>
+      <c r="B33" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8785972602739722</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3">
         <v>2446</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="4">
-        <f t="shared" si="1"/>
-        <v>564.94400000000007</v>
+      <c r="B34" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1426191780821915</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3">
         <v>2077</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="4">
-        <f t="shared" si="1"/>
-        <v>2570.672</v>
+      <c r="B35" s="2">
+        <f t="shared" si="0"/>
+        <v>18.850213698630135</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3">
         <v>9451</v>
       </c>
       <c r="E35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="4">
-        <f t="shared" si="1"/>
-        <v>559.77600000000007</v>
+      <c r="B36" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1047232876712325</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3">
         <v>2058</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="4">
-        <f t="shared" si="1"/>
-        <v>920.72</v>
+        <v>32</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
+        <v>6.7514520547945196</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3">
         <v>3385</v>
       </c>
       <c r="E37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="4">
-        <f t="shared" si="1"/>
-        <v>98.736000000000004</v>
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7240109589041096</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3">
         <v>363</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="4">
-        <f t="shared" si="1"/>
-        <v>486.60800000000006</v>
+      <c r="B39" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5681972602739727</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3">
         <v>1789</v>
       </c>
       <c r="E39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="4">
-        <f t="shared" si="1"/>
-        <v>184.96</v>
+      <c r="B40" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3562739726027395</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3">
         <v>680</v>
       </c>
       <c r="E40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="4">
-        <f t="shared" si="1"/>
-        <v>854.08</v>
+      <c r="B41" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2627945205479456</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3">
         <v>3140</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="4">
-        <f t="shared" si="1"/>
-        <v>435.47200000000004</v>
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1932273972602738</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3">
         <v>1601</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="4">
-        <f t="shared" si="1"/>
-        <v>81.872</v>
+      <c r="B43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.60035068493150678</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3">
         <v>301</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="4">
-        <f t="shared" si="1"/>
-        <v>70.176000000000002</v>
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.51458630136986294</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3">
         <v>258</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="4">
-        <f t="shared" si="1"/>
-        <v>210.52800000000002</v>
+      <c r="B45" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5437589041095889</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3">
         <v>774</v>
       </c>
       <c r="E45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="4">
-        <f t="shared" si="1"/>
-        <v>313.34400000000005</v>
+      <c r="B46" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2976876712328766</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3">
         <v>1152</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="4">
-        <f t="shared" si="1"/>
-        <v>670.20800000000008</v>
+      <c r="B47" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9144986301369862</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3">
         <v>2464</v>
       </c>
       <c r="E47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="4">
-        <f t="shared" si="1"/>
-        <v>1055.3600000000001</v>
+      <c r="B48" s="2">
+        <f t="shared" si="0"/>
+        <v>7.7387397260273971</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3">
         <v>3880</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="4">
-        <f t="shared" si="1"/>
-        <v>562.22400000000005</v>
+      <c r="B49" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1226739726027395</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3">
         <v>2067</v>
       </c>
       <c r="E49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="4">
-        <f t="shared" si="1"/>
-        <v>857.34400000000005</v>
+      <c r="B50" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2867287671232877</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3">
         <v>3152</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="4">
-        <f t="shared" si="1"/>
-        <v>88.128</v>
+      <c r="B51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.64622465753424652</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3">
         <v>324</v>
       </c>
       <c r="E51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="4">
-        <f t="shared" si="1"/>
-        <v>740.928</v>
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>5.4330739726027391</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3">
         <v>2724</v>
       </c>
       <c r="E52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="4">
-        <f t="shared" si="1"/>
-        <v>1564</v>
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>11.468493150684932</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3">
         <v>5750</v>
       </c>
       <c r="E53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="4">
-        <f t="shared" si="1"/>
-        <v>221.40800000000002</v>
+      <c r="B54" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6235397260273972</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3">
         <v>814</v>
       </c>
       <c r="E54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="4">
-        <f t="shared" si="1"/>
-        <v>3008.864</v>
+      <c r="B55" s="2">
+        <f t="shared" si="0"/>
+        <v>22.06338630136986</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3">
         <v>11062</v>
       </c>
       <c r="E55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>